<commit_message>
Fixed the tests with new methods and tables
</commit_message>
<xml_diff>
--- a/tests/data/Metadata.xlsx
+++ b/tests/data/Metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\legregam\Documents\Projets\MSReader\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\legregam\Documents\Projets\MSReader\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4837B991-3B81-4332-9977-CB9D2CBC4142}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F55FE648-A4B5-40A2-A47C-92E535DC7050}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <t>20210426_Blank150_1_12</t>
   </si>
   <si>
-    <t>L</t>
+    <t>µL</t>
   </si>
   <si>
     <t>20210426_Blank150_2_13</t>
@@ -106,7 +106,7 @@
     <t>20210426_WT750_3_26</t>
   </si>
   <si>
-    <t>cell</t>
+    <t>million_cells</t>
   </si>
 </sst>
 </file>
@@ -162,12 +162,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,7 +472,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E2" sqref="E2:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,8 +480,7 @@
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -506,14 +504,14 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2">
-        <v>2.5000000000000001E-5</v>
+      <c r="B2">
+        <v>200</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2">
-        <v>1000000</v>
+        <v>0.6</v>
       </c>
       <c r="E2" t="s">
         <v>28</v>
@@ -523,14 +521,14 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2">
-        <v>2.5000000000000001E-5</v>
+      <c r="B3">
+        <v>200</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3">
-        <v>1000000</v>
+        <v>0.6</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
@@ -540,14 +538,14 @@
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2">
-        <v>2.5000000000000001E-5</v>
+      <c r="B4">
+        <v>200</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4">
-        <v>1000000</v>
+        <v>0.6</v>
       </c>
       <c r="E4" t="s">
         <v>28</v>
@@ -557,14 +555,14 @@
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2">
-        <v>2.5000000000000001E-5</v>
+      <c r="B5">
+        <v>200</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5">
-        <v>1000000</v>
+        <v>0.6</v>
       </c>
       <c r="E5" t="s">
         <v>28</v>
@@ -574,14 +572,14 @@
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2">
-        <v>2.5000000000000001E-5</v>
+      <c r="B6">
+        <v>200</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6">
-        <v>1000000</v>
+        <v>0.6</v>
       </c>
       <c r="E6" t="s">
         <v>28</v>
@@ -591,14 +589,14 @@
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2">
-        <v>2.5000000000000001E-5</v>
+      <c r="B7">
+        <v>200</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7">
-        <v>1000000</v>
+        <v>0.6</v>
       </c>
       <c r="E7" t="s">
         <v>28</v>
@@ -608,14 +606,14 @@
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2">
-        <v>2.5000000000000001E-5</v>
+      <c r="B8">
+        <v>200</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8">
-        <v>1000000</v>
+        <v>0.6</v>
       </c>
       <c r="E8" t="s">
         <v>28</v>
@@ -625,14 +623,14 @@
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2">
-        <v>2.5000000000000001E-5</v>
+      <c r="B9">
+        <v>200</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9">
-        <v>1000000</v>
+        <v>0.6</v>
       </c>
       <c r="E9" t="s">
         <v>28</v>
@@ -642,14 +640,14 @@
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2">
-        <v>2.5000000000000001E-5</v>
+      <c r="B10">
+        <v>200</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10">
-        <v>1000000</v>
+        <v>0.6</v>
       </c>
       <c r="E10" t="s">
         <v>28</v>
@@ -659,14 +657,14 @@
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="2">
-        <v>2.5000000000000001E-5</v>
+      <c r="B11">
+        <v>200</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11">
-        <v>1000000</v>
+        <v>0.6</v>
       </c>
       <c r="E11" t="s">
         <v>28</v>
@@ -676,14 +674,14 @@
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="2">
-        <v>2.5000000000000001E-5</v>
+      <c r="B12">
+        <v>200</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
       </c>
       <c r="D12">
-        <v>1000000</v>
+        <v>0.6</v>
       </c>
       <c r="E12" t="s">
         <v>28</v>
@@ -693,14 +691,14 @@
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="2">
-        <v>2.5000000000000001E-5</v>
+      <c r="B13">
+        <v>200</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
       <c r="D13">
-        <v>1000000</v>
+        <v>0.6</v>
       </c>
       <c r="E13" t="s">
         <v>28</v>
@@ -710,14 +708,14 @@
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="2">
-        <v>2.5000000000000001E-5</v>
+      <c r="B14">
+        <v>200</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
       </c>
       <c r="D14">
-        <v>1000000</v>
+        <v>0.6</v>
       </c>
       <c r="E14" t="s">
         <v>28</v>
@@ -727,14 +725,14 @@
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="2">
-        <v>2.5000000000000001E-5</v>
+      <c r="B15">
+        <v>200</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
       </c>
       <c r="D15">
-        <v>1000000</v>
+        <v>0.6</v>
       </c>
       <c r="E15" t="s">
         <v>28</v>
@@ -744,14 +742,14 @@
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="2">
-        <v>2.5000000000000001E-5</v>
+      <c r="B16">
+        <v>200</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16">
-        <v>1000000</v>
+        <v>0.6</v>
       </c>
       <c r="E16" t="s">
         <v>28</v>
@@ -761,14 +759,14 @@
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="2">
-        <v>2.5000000000000001E-5</v>
+      <c r="B17">
+        <v>200</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
       <c r="D17">
-        <v>1000000</v>
+        <v>0.6</v>
       </c>
       <c r="E17" t="s">
         <v>28</v>
@@ -778,14 +776,14 @@
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="2">
-        <v>2.5000000000000001E-5</v>
+      <c r="B18">
+        <v>200</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
       </c>
       <c r="D18">
-        <v>1000000</v>
+        <v>0.6</v>
       </c>
       <c r="E18" t="s">
         <v>28</v>
@@ -795,14 +793,14 @@
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="2">
-        <v>2.5000000000000001E-5</v>
+      <c r="B19">
+        <v>200</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19">
-        <v>1000000</v>
+        <v>0.6</v>
       </c>
       <c r="E19" t="s">
         <v>28</v>
@@ -812,14 +810,14 @@
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="2">
-        <v>2.5000000000000001E-5</v>
+      <c r="B20">
+        <v>200</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
       </c>
       <c r="D20">
-        <v>1000000</v>
+        <v>0.6</v>
       </c>
       <c r="E20" t="s">
         <v>28</v>
@@ -829,14 +827,14 @@
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="2">
-        <v>2.5000000000000001E-5</v>
+      <c r="B21">
+        <v>200</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="D21">
-        <v>1000000</v>
+        <v>0.6</v>
       </c>
       <c r="E21" t="s">
         <v>28</v>
@@ -846,14 +844,14 @@
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="2">
-        <v>2.5000000000000001E-5</v>
+      <c r="B22">
+        <v>200</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22">
-        <v>1000000</v>
+        <v>0.6</v>
       </c>
       <c r="E22" t="s">
         <v>28</v>
@@ -863,14 +861,14 @@
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="2">
-        <v>2.5000000000000001E-5</v>
+      <c r="B23">
+        <v>200</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23">
-        <v>1000000</v>
+        <v>0.6</v>
       </c>
       <c r="E23" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Fixed tests with new data format and QC values
</commit_message>
<xml_diff>
--- a/tests/data/Metadata.xlsx
+++ b/tests/data/Metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\legregam\Documents\Projets\MSReader\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\legregam\Documents\Projets\MSReader\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F55FE648-A4B5-40A2-A47C-92E535DC7050}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{78A7BDB9-F06C-4D07-B6E9-00717BF19FFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="19">
   <si>
     <t>Sample_Name</t>
   </si>
@@ -37,21 +37,12 @@
     <t>Norm1_Unit</t>
   </si>
   <si>
-    <t>20210426_Blank150_1_12</t>
+    <t>20210426_Cre150_1_20</t>
   </si>
   <si>
     <t>µL</t>
   </si>
   <si>
-    <t>20210426_Blank150_2_13</t>
-  </si>
-  <si>
-    <t>20210426_Blank750_14</t>
-  </si>
-  <si>
-    <t>20210426_Cre150_1_20</t>
-  </si>
-  <si>
     <t>20210426_Cre150_2_21</t>
   </si>
   <si>
@@ -67,27 +58,6 @@
     <t>20210426_Cre750_3_30</t>
   </si>
   <si>
-    <t>20210426_QC_02</t>
-  </si>
-  <si>
-    <t>20210426_SMS01_09</t>
-  </si>
-  <si>
-    <t>20210426_SMS02_08</t>
-  </si>
-  <si>
-    <t>20210426_SMS04_07</t>
-  </si>
-  <si>
-    <t>20210426_SMS08_06</t>
-  </si>
-  <si>
-    <t>20210426_SMS16_05</t>
-  </si>
-  <si>
-    <t>20210426_SMS32_04</t>
-  </si>
-  <si>
     <t>20210426_WT150_1_16</t>
   </si>
   <si>
@@ -106,7 +76,7 @@
     <t>20210426_WT750_3_26</t>
   </si>
   <si>
-    <t>million_cells</t>
+    <t>cell</t>
   </si>
 </sst>
 </file>
@@ -469,18 +439,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E23"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -505,16 +476,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2">
-        <v>0.6</v>
+        <v>100000</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -522,16 +493,16 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3">
-        <v>0.6</v>
+        <v>100000</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -539,16 +510,16 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4">
-        <v>0.6</v>
+        <v>100000</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -556,16 +527,16 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5">
-        <v>0.6</v>
+        <v>100000</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -573,16 +544,16 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6">
-        <v>0.6</v>
+        <v>100000</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -590,16 +561,16 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7">
-        <v>0.6</v>
+        <v>100000</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -607,16 +578,16 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8">
-        <v>0.6</v>
+        <v>100000</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -624,16 +595,16 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9">
-        <v>0.6</v>
+        <v>100000</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -641,16 +612,16 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10">
-        <v>0.6</v>
+        <v>100000</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -658,16 +629,16 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11">
-        <v>0.6</v>
+        <v>100000</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -675,16 +646,16 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
       </c>
       <c r="D12">
-        <v>0.6</v>
+        <v>100000</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -692,186 +663,16 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
       <c r="D13">
-        <v>0.6</v>
+        <v>100000</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14">
-        <v>200</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14">
-        <v>0.6</v>
-      </c>
-      <c r="E14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15">
-        <v>200</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15">
-        <v>0.6</v>
-      </c>
-      <c r="E15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16">
-        <v>200</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16">
-        <v>0.6</v>
-      </c>
-      <c r="E16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17">
-        <v>200</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17">
-        <v>0.6</v>
-      </c>
-      <c r="E17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18">
-        <v>200</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18">
-        <v>0.6</v>
-      </c>
-      <c r="E18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19">
-        <v>200</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19">
-        <v>0.6</v>
-      </c>
-      <c r="E19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20">
-        <v>200</v>
-      </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20">
-        <v>0.6</v>
-      </c>
-      <c r="E20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21">
-        <v>200</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21">
-        <v>0.6</v>
-      </c>
-      <c r="E21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22">
-        <v>200</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22">
-        <v>0.6</v>
-      </c>
-      <c r="E22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23">
-        <v>200</v>
-      </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23">
-        <v>0.6</v>
-      </c>
-      <c r="E23" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added no 13c data handling
</commit_message>
<xml_diff>
--- a/tests/data/Metadata.xlsx
+++ b/tests/data/Metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\legregam\Documents\Projets\MSReader\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\legregam\PycharmProjects\MSReader\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78A7BDB9-F06C-4D07-B6E9-00717BF19FFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E8A77B-2C32-4976-A253-8B50C38B64F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -442,19 +442,19 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D2" sqref="D2:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -488,7 +488,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -505,7 +505,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -522,7 +522,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -539,7 +539,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -556,7 +556,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -573,7 +573,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -590,7 +590,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -607,7 +607,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -624,7 +624,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -641,7 +641,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -658,7 +658,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>